<commit_message>
Doing Updates for Financials
</commit_message>
<xml_diff>
--- a/Financials/Quarterly/AAC_QTR_FIN.xlsx
+++ b/Financials/Quarterly/AAC_QTR_FIN.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Sundeep\Stocks_Automation\Financials\Quarterly\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\sundeep\Stocks_Automation\Financials\Quarterly\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E13C2A3E-92D7-4BB4-8F37-DDD6B9A62EAD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9345"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9348" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AAC" sheetId="6" r:id="rId1"/>
@@ -17,12 +18,12 @@
   <definedNames>
     <definedName name="Ticker">#REF!</definedName>
   </definedNames>
-  <calcPr calcId="152511" calcMode="manual"/>
+  <calcPr calcId="152511" calcMode="manual" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="92">
   <si>
     <t>AAC</t>
   </si>
@@ -303,9 +304,9 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="[$-409]d\-mmm\-yy;@"/>
+    <numFmt numFmtId="164" formatCode="[$-409]d\-mmm\-yy;@"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -347,7 +348,7 @@
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -444,6 +445,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -479,6 +497,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -654,95 +689,102 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A5:K102"/>
+  <dimension ref="A5:L102"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="16.2" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="6" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="69.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="14.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="14.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="16384" width="9.140625" style="1"/>
+    <col min="2" max="2" width="26.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="69.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="14.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="14.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B6" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="C7" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D7" s="2">
+        <v>43373</v>
+      </c>
+      <c r="E7" s="2">
         <v>43281</v>
       </c>
-      <c r="E7" s="2">
+      <c r="F7" s="2">
         <v>43190</v>
       </c>
-      <c r="F7" s="2">
+      <c r="G7" s="2">
         <v>43100</v>
       </c>
-      <c r="G7" s="2">
+      <c r="H7" s="2">
         <v>43008</v>
       </c>
-      <c r="H7" s="2">
+      <c r="I7" s="2">
         <v>42916</v>
       </c>
-      <c r="I7" s="2">
+      <c r="J7" s="2">
         <v>42825</v>
       </c>
-      <c r="J7" s="2">
+      <c r="K7" s="2">
         <v>42735</v>
       </c>
-      <c r="K7" s="2">
+      <c r="L7" s="2">
         <v>42643</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="C8" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D8" s="3">
+        <v>77500</v>
+      </c>
+      <c r="E8" s="3">
         <v>86800</v>
       </c>
-      <c r="E8" s="3">
+      <c r="F8" s="3">
         <v>78500</v>
       </c>
-      <c r="F8" s="3">
+      <c r="G8" s="3">
         <v>86100</v>
       </c>
-      <c r="G8" s="3">
+      <c r="H8" s="3">
         <v>80400</v>
       </c>
-      <c r="H8" s="3">
+      <c r="I8" s="3">
         <v>78000</v>
       </c>
-      <c r="I8" s="3">
+      <c r="J8" s="3">
         <v>73000</v>
       </c>
-      <c r="J8" s="3">
+      <c r="K8" s="3">
         <v>72400</v>
       </c>
-      <c r="K8" s="3">
+      <c r="L8" s="3">
         <v>70500</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="C9" s="1" t="s">
         <v>4</v>
       </c>
@@ -770,8 +812,11 @@
       <c r="K9" s="3" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L9" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="C10" s="1" t="s">
         <v>6</v>
       </c>
@@ -799,8 +844,11 @@
       <c r="K10" s="3" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L10" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="C11" s="1" t="s">
         <v>7</v>
       </c>
@@ -812,8 +860,9 @@
       <c r="I11" s="3"/>
       <c r="J11" s="3"/>
       <c r="K11" s="3"/>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L11" s="3"/>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="C12" s="1" t="s">
         <v>8</v>
       </c>
@@ -841,8 +890,11 @@
       <c r="K12" s="3" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L12" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="C13" s="1" t="s">
         <v>9</v>
       </c>
@@ -870,66 +922,75 @@
       <c r="K13" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L13" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="C14" s="1" t="s">
         <v>10</v>
       </c>
       <c r="D14" s="3">
+        <v>1200</v>
+      </c>
+      <c r="E14" s="3">
         <v>200</v>
       </c>
-      <c r="E14" s="3">
+      <c r="F14" s="3">
         <v>3100</v>
       </c>
-      <c r="F14" s="3">
+      <c r="G14" s="3">
         <v>24200</v>
       </c>
-      <c r="G14" s="3">
+      <c r="H14" s="3">
         <v>400</v>
       </c>
-      <c r="H14" s="3">
+      <c r="I14" s="3">
         <v>5500</v>
       </c>
-      <c r="I14" s="3">
+      <c r="J14" s="3">
         <v>200</v>
       </c>
-      <c r="J14" s="3">
+      <c r="K14" s="3">
         <v>-900</v>
       </c>
-      <c r="K14" s="3">
+      <c r="L14" s="3">
         <v>1400</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="C15" s="1" t="s">
         <v>11</v>
       </c>
       <c r="D15" s="3">
+        <v>5600</v>
+      </c>
+      <c r="E15" s="3">
         <v>5900</v>
       </c>
-      <c r="E15" s="3">
+      <c r="F15" s="3">
         <v>5500</v>
       </c>
-      <c r="F15" s="3">
+      <c r="G15" s="3">
         <v>5800</v>
       </c>
-      <c r="G15" s="3">
+      <c r="H15" s="3">
         <v>5200</v>
       </c>
-      <c r="H15" s="3">
+      <c r="I15" s="3">
         <v>5100</v>
       </c>
-      <c r="I15" s="3">
+      <c r="J15" s="3">
         <v>5500</v>
       </c>
-      <c r="J15" s="3">
+      <c r="K15" s="3">
         <v>4900</v>
       </c>
-      <c r="K15" s="3">
+      <c r="L15" s="3">
         <v>4600</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="D16" s="3"/>
       <c r="E16" s="3"/>
       <c r="F16" s="3"/>
@@ -938,66 +999,73 @@
       <c r="I16" s="3"/>
       <c r="J16" s="3"/>
       <c r="K16" s="3"/>
-    </row>
-    <row r="17" spans="3:11" x14ac:dyDescent="0.2">
+      <c r="L16" s="3"/>
+    </row>
+    <row r="17" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C17" s="1" t="s">
         <v>12</v>
       </c>
       <c r="D17" s="3">
+        <v>84500</v>
+      </c>
+      <c r="E17" s="3">
         <v>84100</v>
       </c>
-      <c r="E17" s="3">
+      <c r="F17" s="3">
         <v>75300</v>
       </c>
-      <c r="F17" s="3">
+      <c r="G17" s="3">
         <v>105100</v>
       </c>
-      <c r="G17" s="3">
+      <c r="H17" s="3">
         <v>75700</v>
       </c>
-      <c r="H17" s="3">
+      <c r="I17" s="3">
         <v>77500</v>
       </c>
-      <c r="I17" s="3">
+      <c r="J17" s="3">
         <v>72500</v>
       </c>
-      <c r="J17" s="3">
+      <c r="K17" s="3">
         <v>72300</v>
       </c>
-      <c r="K17" s="3">
+      <c r="L17" s="3">
         <v>73200</v>
       </c>
     </row>
-    <row r="18" spans="3:11" x14ac:dyDescent="0.2">
+    <row r="18" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C18" s="1" t="s">
         <v>13</v>
       </c>
       <c r="D18" s="3">
+        <v>-7000</v>
+      </c>
+      <c r="E18" s="3">
         <v>2700</v>
       </c>
-      <c r="E18" s="3">
+      <c r="F18" s="3">
         <v>3200</v>
       </c>
-      <c r="F18" s="3">
+      <c r="G18" s="3">
         <v>-19000</v>
       </c>
-      <c r="G18" s="3">
+      <c r="H18" s="3">
         <v>4700</v>
-      </c>
-      <c r="H18" s="3">
-        <v>500</v>
       </c>
       <c r="I18" s="3">
         <v>500</v>
       </c>
       <c r="J18" s="3">
+        <v>500</v>
+      </c>
+      <c r="K18" s="3">
         <v>100</v>
       </c>
-      <c r="K18" s="3">
+      <c r="L18" s="3">
         <v>-2700</v>
       </c>
     </row>
-    <row r="19" spans="3:11" x14ac:dyDescent="0.2">
+    <row r="19" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C19" s="1" t="s">
         <v>14</v>
       </c>
@@ -1009,153 +1077,169 @@
       <c r="I19" s="3"/>
       <c r="J19" s="3"/>
       <c r="K19" s="3"/>
-    </row>
-    <row r="20" spans="3:11" x14ac:dyDescent="0.2">
+      <c r="L19" s="3"/>
+    </row>
+    <row r="20" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C20" s="1" t="s">
         <v>15</v>
       </c>
       <c r="D20" s="3">
+        <v>-800</v>
+      </c>
+      <c r="E20" s="3">
         <v>100</v>
       </c>
-      <c r="E20" s="3">
-        <v>0</v>
-      </c>
       <c r="F20" s="3">
+        <v>0</v>
+      </c>
+      <c r="G20" s="3">
         <v>-200</v>
       </c>
-      <c r="G20" s="3">
-        <v>0</v>
-      </c>
       <c r="H20" s="3">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="I20" s="3">
         <v>100</v>
       </c>
       <c r="J20" s="3">
+        <v>100</v>
+      </c>
+      <c r="K20" s="3">
         <v>300</v>
       </c>
-      <c r="K20" s="3">
+      <c r="L20" s="3">
         <v>-200</v>
       </c>
     </row>
-    <row r="21" spans="3:11" x14ac:dyDescent="0.2">
+    <row r="21" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C21" s="1" t="s">
         <v>16</v>
       </c>
       <c r="D21" s="3">
+        <v>-2200</v>
+      </c>
+      <c r="E21" s="3">
         <v>8700</v>
       </c>
-      <c r="E21" s="3">
+      <c r="F21" s="3">
         <v>8600</v>
       </c>
-      <c r="F21" s="3">
+      <c r="G21" s="3">
         <v>-13500</v>
       </c>
-      <c r="G21" s="3">
+      <c r="H21" s="3">
         <v>9900</v>
       </c>
-      <c r="H21" s="3">
+      <c r="I21" s="3">
         <v>5600</v>
       </c>
-      <c r="I21" s="3">
+      <c r="J21" s="3">
         <v>6100</v>
       </c>
-      <c r="J21" s="3">
+      <c r="K21" s="3">
         <v>5400</v>
       </c>
-      <c r="K21" s="3">
+      <c r="L21" s="3">
         <v>1600</v>
       </c>
     </row>
-    <row r="22" spans="3:11" x14ac:dyDescent="0.2">
+    <row r="22" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C22" s="1" t="s">
         <v>17</v>
       </c>
       <c r="D22" s="3">
+        <v>8700</v>
+      </c>
+      <c r="E22" s="3">
         <v>7900</v>
       </c>
-      <c r="E22" s="3">
+      <c r="F22" s="3">
         <v>6700</v>
-      </c>
-      <c r="F22" s="3">
-        <v>5500</v>
       </c>
       <c r="G22" s="3">
         <v>5500</v>
       </c>
       <c r="H22" s="3">
+        <v>5500</v>
+      </c>
+      <c r="I22" s="3">
         <v>2900</v>
       </c>
-      <c r="I22" s="3">
+      <c r="J22" s="3">
         <v>2800</v>
       </c>
-      <c r="J22" s="3">
+      <c r="K22" s="3">
         <v>2100</v>
       </c>
-      <c r="K22" s="3">
+      <c r="L22" s="3">
         <v>1800</v>
       </c>
     </row>
-    <row r="23" spans="3:11" x14ac:dyDescent="0.2">
+    <row r="23" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C23" s="1" t="s">
         <v>18</v>
       </c>
       <c r="D23" s="3">
+        <v>-16500</v>
+      </c>
+      <c r="E23" s="3">
         <v>-5100</v>
       </c>
-      <c r="E23" s="3">
+      <c r="F23" s="3">
         <v>-3600</v>
       </c>
-      <c r="F23" s="3">
+      <c r="G23" s="3">
         <v>-24700</v>
       </c>
-      <c r="G23" s="3">
+      <c r="H23" s="3">
         <v>-800</v>
       </c>
-      <c r="H23" s="3">
+      <c r="I23" s="3">
         <v>-2300</v>
       </c>
-      <c r="I23" s="3">
+      <c r="J23" s="3">
         <v>-2200</v>
       </c>
-      <c r="J23" s="3">
+      <c r="K23" s="3">
         <v>-1600</v>
       </c>
-      <c r="K23" s="3">
+      <c r="L23" s="3">
         <v>-4800</v>
       </c>
     </row>
-    <row r="24" spans="3:11" x14ac:dyDescent="0.2">
+    <row r="24" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C24" s="1" t="s">
         <v>19</v>
       </c>
       <c r="D24" s="3">
+        <v>-3300</v>
+      </c>
+      <c r="E24" s="3">
         <v>-100</v>
       </c>
-      <c r="E24" s="3">
+      <c r="F24" s="3">
         <v>-1500</v>
       </c>
-      <c r="F24" s="3">
+      <c r="G24" s="3">
         <v>-8100</v>
       </c>
-      <c r="G24" s="3">
+      <c r="H24" s="3">
         <v>-500</v>
       </c>
-      <c r="H24" s="3">
+      <c r="I24" s="3">
         <v>600</v>
       </c>
-      <c r="I24" s="3">
+      <c r="J24" s="3">
         <v>-600</v>
       </c>
-      <c r="J24" s="3">
+      <c r="K24" s="3">
         <v>-300</v>
       </c>
-      <c r="K24" s="3">
+      <c r="L24" s="3">
         <v>-800</v>
       </c>
     </row>
-    <row r="25" spans="3:11" x14ac:dyDescent="0.2">
+    <row r="25" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C25" s="1" t="s">
         <v>20</v>
       </c>
@@ -1183,66 +1267,75 @@
       <c r="K25" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="26" spans="3:11" x14ac:dyDescent="0.2">
+      <c r="L25" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C26" s="1" t="s">
         <v>21</v>
       </c>
       <c r="D26" s="3">
+        <v>-13200</v>
+      </c>
+      <c r="E26" s="3">
         <v>-5000</v>
       </c>
-      <c r="E26" s="3">
+      <c r="F26" s="3">
         <v>-2100</v>
       </c>
-      <c r="F26" s="3">
+      <c r="G26" s="3">
         <v>-16700</v>
       </c>
-      <c r="G26" s="3">
+      <c r="H26" s="3">
         <v>-400</v>
       </c>
-      <c r="H26" s="3">
+      <c r="I26" s="3">
         <v>-2900</v>
       </c>
-      <c r="I26" s="3">
+      <c r="J26" s="3">
         <v>-1600</v>
       </c>
-      <c r="J26" s="3">
+      <c r="K26" s="3">
         <v>-1300</v>
       </c>
-      <c r="K26" s="3">
+      <c r="L26" s="3">
         <v>-4000</v>
       </c>
     </row>
-    <row r="27" spans="3:11" x14ac:dyDescent="0.2">
+    <row r="27" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C27" s="1" t="s">
         <v>22</v>
       </c>
       <c r="D27" s="3">
+        <v>-11500</v>
+      </c>
+      <c r="E27" s="3">
         <v>-3000</v>
       </c>
-      <c r="E27" s="3">
+      <c r="F27" s="3">
         <v>-200</v>
       </c>
-      <c r="F27" s="3">
+      <c r="G27" s="3">
         <v>-15300</v>
       </c>
-      <c r="G27" s="3">
+      <c r="H27" s="3">
         <v>800</v>
       </c>
-      <c r="H27" s="3">
+      <c r="I27" s="3">
         <v>-1900</v>
       </c>
-      <c r="I27" s="3">
+      <c r="J27" s="3">
         <v>-600</v>
       </c>
-      <c r="J27" s="3">
+      <c r="K27" s="3">
         <v>500</v>
       </c>
-      <c r="K27" s="3">
+      <c r="L27" s="3">
         <v>-2500</v>
       </c>
     </row>
-    <row r="28" spans="3:11" x14ac:dyDescent="0.2">
+    <row r="28" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C28" s="1" t="s">
         <v>23</v>
       </c>
@@ -1270,8 +1363,11 @@
       <c r="K28" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="29" spans="3:11" x14ac:dyDescent="0.2">
+      <c r="L28" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C29" s="1" t="s">
         <v>24</v>
       </c>
@@ -1281,11 +1377,11 @@
       <c r="E29" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="F29" s="3">
+      <c r="F29" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G29" s="3">
         <v>-3500</v>
-      </c>
-      <c r="G29" s="3" t="s">
-        <v>5</v>
       </c>
       <c r="H29" s="3" t="s">
         <v>5</v>
@@ -1299,8 +1395,11 @@
       <c r="K29" s="3" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="30" spans="3:11" x14ac:dyDescent="0.2">
+      <c r="L29" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="30" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C30" s="1" t="s">
         <v>25</v>
       </c>
@@ -1328,8 +1427,11 @@
       <c r="K30" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="31" spans="3:11" x14ac:dyDescent="0.2">
+      <c r="L30" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C31" s="1" t="s">
         <v>26</v>
       </c>
@@ -1357,66 +1459,75 @@
       <c r="K31" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="32" spans="3:11" x14ac:dyDescent="0.2">
+      <c r="L31" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C32" s="1" t="s">
         <v>27</v>
       </c>
       <c r="D32" s="3">
+        <v>800</v>
+      </c>
+      <c r="E32" s="3">
         <v>-100</v>
       </c>
-      <c r="E32" s="3">
-        <v>0</v>
-      </c>
       <c r="F32" s="3">
+        <v>0</v>
+      </c>
+      <c r="G32" s="3">
         <v>200</v>
       </c>
-      <c r="G32" s="3">
-        <v>0</v>
-      </c>
       <c r="H32" s="3">
-        <v>-100</v>
+        <v>0</v>
       </c>
       <c r="I32" s="3">
         <v>-100</v>
       </c>
       <c r="J32" s="3">
+        <v>-100</v>
+      </c>
+      <c r="K32" s="3">
         <v>-300</v>
       </c>
-      <c r="K32" s="3">
+      <c r="L32" s="3">
         <v>200</v>
       </c>
     </row>
-    <row r="33" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="33" spans="2:12" x14ac:dyDescent="0.3">
       <c r="C33" s="1" t="s">
         <v>28</v>
       </c>
       <c r="D33" s="3">
+        <v>-11500</v>
+      </c>
+      <c r="E33" s="3">
         <v>-3000</v>
       </c>
-      <c r="E33" s="3">
+      <c r="F33" s="3">
         <v>-200</v>
       </c>
-      <c r="F33" s="3">
+      <c r="G33" s="3">
         <v>-18800</v>
       </c>
-      <c r="G33" s="3">
+      <c r="H33" s="3">
         <v>800</v>
       </c>
-      <c r="H33" s="3">
+      <c r="I33" s="3">
         <v>-1900</v>
       </c>
-      <c r="I33" s="3">
+      <c r="J33" s="3">
         <v>-600</v>
       </c>
-      <c r="J33" s="3">
+      <c r="K33" s="3">
         <v>500</v>
       </c>
-      <c r="K33" s="3">
+      <c r="L33" s="3">
         <v>-2500</v>
       </c>
     </row>
-    <row r="34" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:12" x14ac:dyDescent="0.3">
       <c r="C34" s="1" t="s">
         <v>29</v>
       </c>
@@ -1444,71 +1555,80 @@
       <c r="K34" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="35" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="L34" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="2:12" x14ac:dyDescent="0.3">
       <c r="C35" s="1" t="s">
         <v>30</v>
       </c>
       <c r="D35" s="3">
+        <v>-11500</v>
+      </c>
+      <c r="E35" s="3">
         <v>-3000</v>
       </c>
-      <c r="E35" s="3">
+      <c r="F35" s="3">
         <v>-200</v>
       </c>
-      <c r="F35" s="3">
+      <c r="G35" s="3">
         <v>-18800</v>
       </c>
-      <c r="G35" s="3">
+      <c r="H35" s="3">
         <v>800</v>
       </c>
-      <c r="H35" s="3">
+      <c r="I35" s="3">
         <v>-1900</v>
       </c>
-      <c r="I35" s="3">
+      <c r="J35" s="3">
         <v>-600</v>
       </c>
-      <c r="J35" s="3">
+      <c r="K35" s="3">
         <v>500</v>
       </c>
-      <c r="K35" s="3">
+      <c r="L35" s="3">
         <v>-2500</v>
       </c>
     </row>
-    <row r="37" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="37" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B37" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="38" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="38" spans="2:12" x14ac:dyDescent="0.3">
       <c r="C38" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D38" s="2">
+        <v>43373</v>
+      </c>
+      <c r="E38" s="2">
         <v>43281</v>
       </c>
-      <c r="E38" s="2">
+      <c r="F38" s="2">
         <v>43190</v>
       </c>
-      <c r="F38" s="2">
+      <c r="G38" s="2">
         <v>43100</v>
       </c>
-      <c r="G38" s="2">
+      <c r="H38" s="2">
         <v>43008</v>
       </c>
-      <c r="H38" s="2">
+      <c r="I38" s="2">
         <v>42916</v>
       </c>
-      <c r="I38" s="2">
+      <c r="J38" s="2">
         <v>42825</v>
       </c>
-      <c r="J38" s="2">
+      <c r="K38" s="2">
         <v>42735</v>
       </c>
-      <c r="K38" s="2">
+      <c r="L38" s="2">
         <v>42643</v>
       </c>
     </row>
-    <row r="39" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="39" spans="2:12" x14ac:dyDescent="0.3">
       <c r="C39" s="1" t="s">
         <v>32</v>
       </c>
@@ -1520,8 +1640,9 @@
       <c r="I39" s="3"/>
       <c r="J39" s="3"/>
       <c r="K39" s="3"/>
-    </row>
-    <row r="40" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="L39" s="3"/>
+    </row>
+    <row r="40" spans="2:12" x14ac:dyDescent="0.3">
       <c r="C40" s="1" t="s">
         <v>33</v>
       </c>
@@ -1533,37 +1654,41 @@
       <c r="I40" s="3"/>
       <c r="J40" s="3"/>
       <c r="K40" s="3"/>
-    </row>
-    <row r="41" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="L40" s="3"/>
+    </row>
+    <row r="41" spans="2:12" x14ac:dyDescent="0.3">
       <c r="C41" s="1" t="s">
         <v>34</v>
       </c>
       <c r="D41" s="3">
+        <v>5300</v>
+      </c>
+      <c r="E41" s="3">
         <v>11400</v>
       </c>
-      <c r="E41" s="3">
+      <c r="F41" s="3">
         <v>14300</v>
       </c>
-      <c r="F41" s="3">
+      <c r="G41" s="3">
         <v>13800</v>
       </c>
-      <c r="G41" s="3">
+      <c r="H41" s="3">
         <v>16400</v>
       </c>
-      <c r="H41" s="3">
+      <c r="I41" s="3">
         <v>10800</v>
       </c>
-      <c r="I41" s="3">
+      <c r="J41" s="3">
         <v>5900</v>
       </c>
-      <c r="J41" s="3">
+      <c r="K41" s="3">
         <v>4000</v>
       </c>
-      <c r="K41" s="3">
+      <c r="L41" s="3">
         <v>13300</v>
       </c>
     </row>
-    <row r="42" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="42" spans="2:12" x14ac:dyDescent="0.3">
       <c r="C42" s="1" t="s">
         <v>35</v>
       </c>
@@ -1591,37 +1716,43 @@
       <c r="K42" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="43" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="L42" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="2:12" x14ac:dyDescent="0.3">
       <c r="C43" s="1" t="s">
         <v>36</v>
       </c>
       <c r="D43" s="3">
+        <v>94600</v>
+      </c>
+      <c r="E43" s="3">
         <v>97400</v>
       </c>
-      <c r="E43" s="3">
+      <c r="F43" s="3">
         <v>99600</v>
       </c>
-      <c r="F43" s="3">
+      <c r="G43" s="3">
         <v>94100</v>
       </c>
-      <c r="G43" s="3">
+      <c r="H43" s="3">
         <v>92500</v>
       </c>
-      <c r="H43" s="3">
+      <c r="I43" s="3">
         <v>96500</v>
       </c>
-      <c r="I43" s="3">
+      <c r="J43" s="3">
         <v>94100</v>
       </c>
-      <c r="J43" s="3">
+      <c r="K43" s="3">
         <v>87300</v>
       </c>
-      <c r="K43" s="3">
+      <c r="L43" s="3">
         <v>80400</v>
       </c>
     </row>
-    <row r="44" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="44" spans="2:12" x14ac:dyDescent="0.3">
       <c r="C44" s="1" t="s">
         <v>37</v>
       </c>
@@ -1649,66 +1780,75 @@
       <c r="K44" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="45" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="L44" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="2:12" x14ac:dyDescent="0.3">
       <c r="C45" s="1" t="s">
         <v>38</v>
       </c>
       <c r="D45" s="3">
+        <v>5500</v>
+      </c>
+      <c r="E45" s="3">
         <v>4600</v>
       </c>
-      <c r="E45" s="3">
+      <c r="F45" s="3">
         <v>3400</v>
       </c>
-      <c r="F45" s="3">
+      <c r="G45" s="3">
         <v>4000</v>
       </c>
-      <c r="G45" s="3">
+      <c r="H45" s="3">
         <v>6000</v>
       </c>
-      <c r="H45" s="3">
+      <c r="I45" s="3">
         <v>4500</v>
       </c>
-      <c r="I45" s="3">
+      <c r="J45" s="3">
         <v>4900</v>
       </c>
-      <c r="J45" s="3">
+      <c r="K45" s="3">
         <v>5200</v>
       </c>
-      <c r="K45" s="3">
+      <c r="L45" s="3">
         <v>3200</v>
       </c>
     </row>
-    <row r="46" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="46" spans="2:12" x14ac:dyDescent="0.3">
       <c r="C46" s="1" t="s">
         <v>39</v>
       </c>
       <c r="D46" s="3">
+        <v>105400</v>
+      </c>
+      <c r="E46" s="3">
         <v>113400</v>
       </c>
-      <c r="E46" s="3">
+      <c r="F46" s="3">
         <v>117300</v>
       </c>
-      <c r="F46" s="3">
+      <c r="G46" s="3">
         <v>111900</v>
       </c>
-      <c r="G46" s="3">
+      <c r="H46" s="3">
         <v>115000</v>
       </c>
-      <c r="H46" s="3">
+      <c r="I46" s="3">
         <v>111800</v>
       </c>
-      <c r="I46" s="3">
+      <c r="J46" s="3">
         <v>104900</v>
       </c>
-      <c r="J46" s="3">
+      <c r="K46" s="3">
         <v>96500</v>
       </c>
-      <c r="K46" s="3">
+      <c r="L46" s="3">
         <v>96900</v>
       </c>
     </row>
-    <row r="47" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="47" spans="2:12" x14ac:dyDescent="0.3">
       <c r="C47" s="1" t="s">
         <v>40</v>
       </c>
@@ -1736,66 +1876,75 @@
       <c r="K47" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="48" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="L47" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="2:12" x14ac:dyDescent="0.3">
       <c r="C48" s="1" t="s">
         <v>41</v>
       </c>
       <c r="D48" s="3">
+        <v>166300</v>
+      </c>
+      <c r="E48" s="3">
         <v>168400</v>
       </c>
-      <c r="E48" s="3">
+      <c r="F48" s="3">
         <v>169700</v>
       </c>
-      <c r="F48" s="3">
+      <c r="G48" s="3">
         <v>152500</v>
       </c>
-      <c r="G48" s="3">
+      <c r="H48" s="3">
         <v>151800</v>
       </c>
-      <c r="H48" s="3">
+      <c r="I48" s="3">
         <v>149000</v>
       </c>
-      <c r="I48" s="3">
+      <c r="J48" s="3">
         <v>145400</v>
       </c>
-      <c r="J48" s="3">
+      <c r="K48" s="3">
         <v>141300</v>
       </c>
-      <c r="K48" s="3">
+      <c r="L48" s="3">
         <v>136200</v>
       </c>
     </row>
-    <row r="49" spans="3:11" x14ac:dyDescent="0.2">
+    <row r="49" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C49" s="1" t="s">
         <v>42</v>
       </c>
       <c r="D49" s="3">
+        <v>211500</v>
+      </c>
+      <c r="E49" s="3">
         <v>210400</v>
       </c>
-      <c r="E49" s="3">
+      <c r="F49" s="3">
         <v>210900</v>
       </c>
-      <c r="F49" s="3">
+      <c r="G49" s="3">
         <v>143200</v>
       </c>
-      <c r="G49" s="3">
+      <c r="H49" s="3">
         <v>143600</v>
       </c>
-      <c r="H49" s="3">
+      <c r="I49" s="3">
         <v>143900</v>
       </c>
-      <c r="I49" s="3">
+      <c r="J49" s="3">
         <v>144300</v>
       </c>
-      <c r="J49" s="3">
+      <c r="K49" s="3">
         <v>144800</v>
       </c>
-      <c r="K49" s="3">
+      <c r="L49" s="3">
         <v>145400</v>
       </c>
     </row>
-    <row r="50" spans="3:11" x14ac:dyDescent="0.2">
+    <row r="50" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C50" s="1" t="s">
         <v>43</v>
       </c>
@@ -1823,8 +1972,11 @@
       <c r="K50" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="51" spans="3:11" x14ac:dyDescent="0.2">
+      <c r="L50" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C51" s="1" t="s">
         <v>44</v>
       </c>
@@ -1852,37 +2004,43 @@
       <c r="K51" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="52" spans="3:11" x14ac:dyDescent="0.2">
+      <c r="L51" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C52" s="1" t="s">
         <v>45</v>
       </c>
       <c r="D52" s="3">
+        <v>23700</v>
+      </c>
+      <c r="E52" s="3">
         <v>20600</v>
       </c>
-      <c r="E52" s="3">
+      <c r="F52" s="3">
         <v>21500</v>
       </c>
-      <c r="F52" s="3">
+      <c r="G52" s="3">
         <v>20600</v>
       </c>
-      <c r="G52" s="3">
+      <c r="H52" s="3">
         <v>7200</v>
       </c>
-      <c r="H52" s="3">
+      <c r="I52" s="3">
         <v>2000</v>
       </c>
-      <c r="I52" s="3">
+      <c r="J52" s="3">
         <v>1900</v>
       </c>
-      <c r="J52" s="3">
+      <c r="K52" s="3">
         <v>1300</v>
       </c>
-      <c r="K52" s="3">
+      <c r="L52" s="3">
         <v>1800</v>
       </c>
     </row>
-    <row r="53" spans="3:11" x14ac:dyDescent="0.2">
+    <row r="53" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C53" s="1" t="s">
         <v>46</v>
       </c>
@@ -1910,37 +2068,43 @@
       <c r="K53" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="54" spans="3:11" x14ac:dyDescent="0.2">
+      <c r="L53" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C54" s="1" t="s">
         <v>47</v>
       </c>
       <c r="D54" s="3">
+        <v>507000</v>
+      </c>
+      <c r="E54" s="3">
         <v>512800</v>
       </c>
-      <c r="E54" s="3">
+      <c r="F54" s="3">
         <v>519400</v>
       </c>
-      <c r="F54" s="3">
+      <c r="G54" s="3">
         <v>428300</v>
       </c>
-      <c r="G54" s="3">
+      <c r="H54" s="3">
         <v>417600</v>
       </c>
-      <c r="H54" s="3">
+      <c r="I54" s="3">
         <v>406700</v>
       </c>
-      <c r="I54" s="3">
+      <c r="J54" s="3">
         <v>396600</v>
       </c>
-      <c r="J54" s="3">
+      <c r="K54" s="3">
         <v>383900</v>
       </c>
-      <c r="K54" s="3">
+      <c r="L54" s="3">
         <v>380300</v>
       </c>
     </row>
-    <row r="55" spans="3:11" x14ac:dyDescent="0.2">
+    <row r="55" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C55" s="1" t="s">
         <v>48</v>
       </c>
@@ -1952,8 +2116,9 @@
       <c r="I55" s="3"/>
       <c r="J55" s="3"/>
       <c r="K55" s="3"/>
-    </row>
-    <row r="56" spans="3:11" x14ac:dyDescent="0.2">
+      <c r="L55" s="3"/>
+    </row>
+    <row r="56" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C56" s="1" t="s">
         <v>49</v>
       </c>
@@ -1965,182 +2130,201 @@
       <c r="I56" s="3"/>
       <c r="J56" s="3"/>
       <c r="K56" s="3"/>
-    </row>
-    <row r="57" spans="3:11" x14ac:dyDescent="0.2">
+      <c r="L56" s="3"/>
+    </row>
+    <row r="57" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C57" s="1" t="s">
         <v>50</v>
       </c>
       <c r="D57" s="3">
+        <v>8700</v>
+      </c>
+      <c r="E57" s="3">
         <v>6600</v>
       </c>
-      <c r="E57" s="3">
+      <c r="F57" s="3">
         <v>3300</v>
       </c>
-      <c r="F57" s="3">
+      <c r="G57" s="3">
         <v>4600</v>
       </c>
-      <c r="G57" s="3">
+      <c r="H57" s="3">
         <v>5700</v>
       </c>
-      <c r="H57" s="3">
+      <c r="I57" s="3">
         <v>10400</v>
       </c>
-      <c r="I57" s="3">
+      <c r="J57" s="3">
         <v>13700</v>
       </c>
-      <c r="J57" s="3">
+      <c r="K57" s="3">
         <v>9200</v>
       </c>
-      <c r="K57" s="3">
+      <c r="L57" s="3">
         <v>10300</v>
       </c>
     </row>
-    <row r="58" spans="3:11" x14ac:dyDescent="0.2">
+    <row r="58" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C58" s="1" t="s">
         <v>51</v>
       </c>
       <c r="D58" s="3">
+        <v>8400</v>
+      </c>
+      <c r="E58" s="3">
         <v>6700</v>
       </c>
-      <c r="E58" s="3">
+      <c r="F58" s="3">
         <v>7300</v>
-      </c>
-      <c r="F58" s="3">
-        <v>4700</v>
       </c>
       <c r="G58" s="3">
         <v>4700</v>
       </c>
       <c r="H58" s="3">
+        <v>4700</v>
+      </c>
+      <c r="I58" s="3">
         <v>4500</v>
       </c>
-      <c r="I58" s="3">
+      <c r="J58" s="3">
         <v>11000</v>
       </c>
-      <c r="J58" s="3">
+      <c r="K58" s="3">
         <v>9400</v>
       </c>
-      <c r="K58" s="3">
+      <c r="L58" s="3">
         <v>8600</v>
       </c>
     </row>
-    <row r="59" spans="3:11" x14ac:dyDescent="0.2">
+    <row r="59" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C59" s="1" t="s">
         <v>52</v>
       </c>
       <c r="D59" s="3">
+        <v>31600</v>
+      </c>
+      <c r="E59" s="3">
         <v>30500</v>
       </c>
-      <c r="E59" s="3">
+      <c r="F59" s="3">
         <v>35000</v>
       </c>
-      <c r="F59" s="3">
+      <c r="G59" s="3">
         <v>51300</v>
       </c>
-      <c r="G59" s="3">
+      <c r="H59" s="3">
         <v>24600</v>
       </c>
-      <c r="H59" s="3">
+      <c r="I59" s="3">
         <v>24800</v>
       </c>
-      <c r="I59" s="3">
+      <c r="J59" s="3">
         <v>24900</v>
       </c>
-      <c r="J59" s="3">
+      <c r="K59" s="3">
         <v>26700</v>
       </c>
-      <c r="K59" s="3">
+      <c r="L59" s="3">
         <v>21300</v>
       </c>
     </row>
-    <row r="60" spans="3:11" x14ac:dyDescent="0.2">
+    <row r="60" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C60" s="1" t="s">
         <v>53</v>
       </c>
       <c r="D60" s="3">
+        <v>48700</v>
+      </c>
+      <c r="E60" s="3">
         <v>43800</v>
       </c>
-      <c r="E60" s="3">
+      <c r="F60" s="3">
         <v>45700</v>
       </c>
-      <c r="F60" s="3">
+      <c r="G60" s="3">
         <v>60600</v>
       </c>
-      <c r="G60" s="3">
+      <c r="H60" s="3">
         <v>35100</v>
       </c>
-      <c r="H60" s="3">
+      <c r="I60" s="3">
         <v>39700</v>
       </c>
-      <c r="I60" s="3">
+      <c r="J60" s="3">
         <v>49500</v>
       </c>
-      <c r="J60" s="3">
+      <c r="K60" s="3">
         <v>45300</v>
       </c>
-      <c r="K60" s="3">
+      <c r="L60" s="3">
         <v>40200</v>
       </c>
     </row>
-    <row r="61" spans="3:11" x14ac:dyDescent="0.2">
+    <row r="61" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C61" s="1" t="s">
         <v>54</v>
       </c>
       <c r="D61" s="3">
+        <v>321600</v>
+      </c>
+      <c r="E61" s="3">
         <v>319800</v>
       </c>
-      <c r="E61" s="3">
+      <c r="F61" s="3">
         <v>321000</v>
       </c>
-      <c r="F61" s="3">
+      <c r="G61" s="3">
         <v>221000</v>
       </c>
-      <c r="G61" s="3">
+      <c r="H61" s="3">
         <v>222300</v>
       </c>
-      <c r="H61" s="3">
+      <c r="I61" s="3">
         <v>208500</v>
       </c>
-      <c r="I61" s="3">
+      <c r="J61" s="3">
         <v>187500</v>
       </c>
-      <c r="J61" s="3">
+      <c r="K61" s="3">
         <v>179700</v>
       </c>
-      <c r="K61" s="3">
+      <c r="L61" s="3">
         <v>180800</v>
       </c>
     </row>
-    <row r="62" spans="3:11" x14ac:dyDescent="0.2">
+    <row r="62" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C62" s="1" t="s">
         <v>55</v>
       </c>
       <c r="D62" s="3">
-        <v>12300</v>
+        <v>12000</v>
       </c>
       <c r="E62" s="3">
         <v>12300</v>
       </c>
       <c r="F62" s="3">
+        <v>12300</v>
+      </c>
+      <c r="G62" s="3">
         <v>10500</v>
-      </c>
-      <c r="G62" s="3">
-        <v>3800</v>
       </c>
       <c r="H62" s="3">
         <v>3800</v>
       </c>
       <c r="I62" s="3">
-        <v>4100</v>
+        <v>3800</v>
       </c>
       <c r="J62" s="3">
         <v>4100</v>
       </c>
       <c r="K62" s="3">
+        <v>4100</v>
+      </c>
+      <c r="L62" s="3">
         <v>4300</v>
       </c>
     </row>
-    <row r="63" spans="3:11" x14ac:dyDescent="0.2">
+    <row r="63" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C63" s="1" t="s">
         <v>56</v>
       </c>
@@ -2168,8 +2352,11 @@
       <c r="K63" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="64" spans="3:11" x14ac:dyDescent="0.2">
+      <c r="L63" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C64" s="1" t="s">
         <v>20</v>
       </c>
@@ -2197,8 +2384,11 @@
       <c r="K64" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="65" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="L64" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="2:12" x14ac:dyDescent="0.3">
       <c r="C65" s="1" t="s">
         <v>57</v>
       </c>
@@ -2226,37 +2416,43 @@
       <c r="K65" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="66" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="L65" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="2:12" x14ac:dyDescent="0.3">
       <c r="C66" s="1" t="s">
         <v>58</v>
       </c>
       <c r="D66" s="3">
+        <v>361900</v>
+      </c>
+      <c r="E66" s="3">
         <v>357200</v>
       </c>
-      <c r="E66" s="3">
+      <c r="F66" s="3">
         <v>362200</v>
       </c>
-      <c r="F66" s="3">
+      <c r="G66" s="3">
         <v>277300</v>
       </c>
-      <c r="G66" s="3">
+      <c r="H66" s="3">
         <v>247700</v>
       </c>
-      <c r="H66" s="3">
+      <c r="I66" s="3">
         <v>239700</v>
       </c>
-      <c r="I66" s="3">
+      <c r="J66" s="3">
         <v>229800</v>
       </c>
-      <c r="J66" s="3">
+      <c r="K66" s="3">
         <v>218800</v>
       </c>
-      <c r="K66" s="3">
+      <c r="L66" s="3">
         <v>216800</v>
       </c>
     </row>
-    <row r="67" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="67" spans="2:12" x14ac:dyDescent="0.3">
       <c r="C67" s="1" t="s">
         <v>59</v>
       </c>
@@ -2268,8 +2464,9 @@
       <c r="I67" s="3"/>
       <c r="J67" s="3"/>
       <c r="K67" s="3"/>
-    </row>
-    <row r="68" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="L67" s="3"/>
+    </row>
+    <row r="68" spans="2:12" x14ac:dyDescent="0.3">
       <c r="C68" s="1" t="s">
         <v>60</v>
       </c>
@@ -2297,8 +2494,11 @@
       <c r="K68" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="69" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="L68" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="2:12" x14ac:dyDescent="0.3">
       <c r="C69" s="1" t="s">
         <v>61</v>
       </c>
@@ -2326,8 +2526,11 @@
       <c r="K69" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="70" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="L69" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="2:12" x14ac:dyDescent="0.3">
       <c r="C70" s="1" t="s">
         <v>62</v>
       </c>
@@ -2355,8 +2558,11 @@
       <c r="K70" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="71" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="L70" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="2:12" x14ac:dyDescent="0.3">
       <c r="C71" s="1" t="s">
         <v>63</v>
       </c>
@@ -2384,37 +2590,43 @@
       <c r="K71" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="72" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="L71" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="2:12" x14ac:dyDescent="0.3">
       <c r="C72" s="1" t="s">
         <v>64</v>
       </c>
       <c r="D72" s="3">
+        <v>-16200</v>
+      </c>
+      <c r="E72" s="3">
         <v>-4700</v>
       </c>
-      <c r="E72" s="3">
+      <c r="F72" s="3">
         <v>-1700</v>
       </c>
-      <c r="F72" s="3">
+      <c r="G72" s="3">
         <v>-1500</v>
       </c>
-      <c r="G72" s="3">
+      <c r="H72" s="3">
         <v>17400</v>
       </c>
-      <c r="H72" s="3">
+      <c r="I72" s="3">
         <v>16600</v>
       </c>
-      <c r="I72" s="3">
+      <c r="J72" s="3">
         <v>18500</v>
       </c>
-      <c r="J72" s="3">
+      <c r="K72" s="3">
         <v>19100</v>
       </c>
-      <c r="K72" s="3">
+      <c r="L72" s="3">
         <v>18600</v>
       </c>
     </row>
-    <row r="73" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="73" spans="2:12" x14ac:dyDescent="0.3">
       <c r="C73" s="1" t="s">
         <v>65</v>
       </c>
@@ -2442,8 +2654,11 @@
       <c r="K73" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="74" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="L73" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="2:12" x14ac:dyDescent="0.3">
       <c r="C74" s="1" t="s">
         <v>66</v>
       </c>
@@ -2471,8 +2686,11 @@
       <c r="K74" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="75" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="L74" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="2:12" x14ac:dyDescent="0.3">
       <c r="C75" s="1" t="s">
         <v>67</v>
       </c>
@@ -2500,37 +2718,43 @@
       <c r="K75" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="76" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="L75" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="2:12" x14ac:dyDescent="0.3">
       <c r="C76" s="1" t="s">
         <v>68</v>
       </c>
       <c r="D76" s="3">
+        <v>145100</v>
+      </c>
+      <c r="E76" s="3">
         <v>155500</v>
       </c>
-      <c r="E76" s="3">
+      <c r="F76" s="3">
         <v>157200</v>
       </c>
-      <c r="F76" s="3">
+      <c r="G76" s="3">
         <v>151000</v>
       </c>
-      <c r="G76" s="3">
+      <c r="H76" s="3">
         <v>169800</v>
       </c>
-      <c r="H76" s="3">
+      <c r="I76" s="3">
         <v>167000</v>
       </c>
-      <c r="I76" s="3">
+      <c r="J76" s="3">
         <v>166900</v>
       </c>
-      <c r="J76" s="3">
+      <c r="K76" s="3">
         <v>165100</v>
       </c>
-      <c r="K76" s="3">
+      <c r="L76" s="3">
         <v>163500</v>
       </c>
     </row>
-    <row r="77" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="77" spans="2:12" x14ac:dyDescent="0.3">
       <c r="C77" s="1" t="s">
         <v>69</v>
       </c>
@@ -2558,71 +2782,80 @@
       <c r="K77" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="79" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="L77" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B79" s="1" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="80" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="80" spans="2:12" x14ac:dyDescent="0.3">
       <c r="C80" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D80" s="2">
+        <v>43373</v>
+      </c>
+      <c r="E80" s="2">
         <v>43281</v>
       </c>
-      <c r="E80" s="2">
+      <c r="F80" s="2">
         <v>43190</v>
       </c>
-      <c r="F80" s="2">
+      <c r="G80" s="2">
         <v>43100</v>
       </c>
-      <c r="G80" s="2">
+      <c r="H80" s="2">
         <v>43008</v>
       </c>
-      <c r="H80" s="2">
+      <c r="I80" s="2">
         <v>42916</v>
       </c>
-      <c r="I80" s="2">
+      <c r="J80" s="2">
         <v>42825</v>
       </c>
-      <c r="J80" s="2">
+      <c r="K80" s="2">
         <v>42735</v>
       </c>
-      <c r="K80" s="2">
+      <c r="L80" s="2">
         <v>42643</v>
       </c>
     </row>
-    <row r="81" spans="3:11" x14ac:dyDescent="0.2">
+    <row r="81" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C81" s="1" t="s">
         <v>28</v>
       </c>
       <c r="D81" s="3">
+        <v>-11500</v>
+      </c>
+      <c r="E81" s="3">
         <v>-3000</v>
       </c>
-      <c r="E81" s="3">
+      <c r="F81" s="3">
         <v>-200</v>
       </c>
-      <c r="F81" s="3">
+      <c r="G81" s="3">
         <v>-18800</v>
       </c>
-      <c r="G81" s="3">
+      <c r="H81" s="3">
         <v>800</v>
       </c>
-      <c r="H81" s="3">
+      <c r="I81" s="3">
         <v>-1900</v>
       </c>
-      <c r="I81" s="3">
+      <c r="J81" s="3">
         <v>-600</v>
       </c>
-      <c r="J81" s="3">
+      <c r="K81" s="3">
         <v>500</v>
       </c>
-      <c r="K81" s="3">
+      <c r="L81" s="3">
         <v>-2500</v>
       </c>
     </row>
-    <row r="82" spans="3:11" x14ac:dyDescent="0.2">
+    <row r="82" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C82" s="1" t="s">
         <v>71</v>
       </c>
@@ -2634,37 +2867,41 @@
       <c r="I82" s="3"/>
       <c r="J82" s="3"/>
       <c r="K82" s="3"/>
-    </row>
-    <row r="83" spans="3:11" x14ac:dyDescent="0.2">
+      <c r="L82" s="3"/>
+    </row>
+    <row r="83" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C83" s="1" t="s">
         <v>72</v>
       </c>
       <c r="D83" s="3">
+        <v>5600</v>
+      </c>
+      <c r="E83" s="3">
         <v>5900</v>
       </c>
-      <c r="E83" s="3">
+      <c r="F83" s="3">
         <v>5500</v>
       </c>
-      <c r="F83" s="3">
+      <c r="G83" s="3">
         <v>5800</v>
       </c>
-      <c r="G83" s="3">
+      <c r="H83" s="3">
         <v>5200</v>
       </c>
-      <c r="H83" s="3">
+      <c r="I83" s="3">
         <v>5100</v>
       </c>
-      <c r="I83" s="3">
+      <c r="J83" s="3">
         <v>5500</v>
       </c>
-      <c r="J83" s="3">
+      <c r="K83" s="3">
         <v>4900</v>
       </c>
-      <c r="K83" s="3">
+      <c r="L83" s="3">
         <v>4600</v>
       </c>
     </row>
-    <row r="84" spans="3:11" x14ac:dyDescent="0.2">
+    <row r="84" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C84" s="1" t="s">
         <v>73</v>
       </c>
@@ -2692,8 +2929,11 @@
       <c r="K84" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="85" spans="3:11" x14ac:dyDescent="0.2">
+      <c r="L84" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C85" s="1" t="s">
         <v>74</v>
       </c>
@@ -2721,8 +2961,11 @@
       <c r="K85" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="86" spans="3:11" x14ac:dyDescent="0.2">
+      <c r="L85" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C86" s="1" t="s">
         <v>75</v>
       </c>
@@ -2750,8 +2993,11 @@
       <c r="K86" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="87" spans="3:11" x14ac:dyDescent="0.2">
+      <c r="L86" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C87" s="1" t="s">
         <v>76</v>
       </c>
@@ -2779,8 +3025,11 @@
       <c r="K87" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="88" spans="3:11" x14ac:dyDescent="0.2">
+      <c r="L87" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C88" s="1" t="s">
         <v>77</v>
       </c>
@@ -2808,37 +3057,43 @@
       <c r="K88" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="89" spans="3:11" x14ac:dyDescent="0.2">
+      <c r="L88" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C89" s="1" t="s">
         <v>78</v>
       </c>
       <c r="D89" s="3">
+        <v>-4000</v>
+      </c>
+      <c r="E89" s="3">
         <v>3300</v>
       </c>
-      <c r="E89" s="3">
+      <c r="F89" s="3">
         <v>-19000</v>
       </c>
-      <c r="F89" s="3">
+      <c r="G89" s="3">
         <v>5300</v>
       </c>
-      <c r="G89" s="3">
+      <c r="H89" s="3">
         <v>5600</v>
       </c>
-      <c r="H89" s="3">
+      <c r="I89" s="3">
         <v>4000</v>
       </c>
-      <c r="I89" s="3">
+      <c r="J89" s="3">
         <v>4400</v>
       </c>
-      <c r="J89" s="3">
+      <c r="K89" s="3">
         <v>-1200</v>
       </c>
-      <c r="K89" s="3">
+      <c r="L89" s="3">
         <v>-5000</v>
       </c>
     </row>
-    <row r="90" spans="3:11" x14ac:dyDescent="0.2">
+    <row r="90" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C90" s="1" t="s">
         <v>79</v>
       </c>
@@ -2850,37 +3105,41 @@
       <c r="I90" s="3"/>
       <c r="J90" s="3"/>
       <c r="K90" s="3"/>
-    </row>
-    <row r="91" spans="3:11" x14ac:dyDescent="0.2">
+      <c r="L90" s="3"/>
+    </row>
+    <row r="91" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C91" s="1" t="s">
         <v>80</v>
       </c>
       <c r="D91" s="3">
+        <v>-4300</v>
+      </c>
+      <c r="E91" s="3">
         <v>-3900</v>
       </c>
-      <c r="E91" s="3">
+      <c r="F91" s="3">
         <v>-7300</v>
       </c>
-      <c r="F91" s="3">
+      <c r="G91" s="3">
         <v>-5900</v>
       </c>
-      <c r="G91" s="3">
+      <c r="H91" s="3">
         <v>-8500</v>
       </c>
-      <c r="H91" s="3">
+      <c r="I91" s="3">
         <v>-8000</v>
       </c>
-      <c r="I91" s="3">
+      <c r="J91" s="3">
         <v>-10700</v>
       </c>
-      <c r="J91" s="3">
+      <c r="K91" s="3">
         <v>-7300</v>
       </c>
-      <c r="K91" s="3">
+      <c r="L91" s="3">
         <v>-10200</v>
       </c>
     </row>
-    <row r="92" spans="3:11" x14ac:dyDescent="0.2">
+    <row r="92" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C92" s="1" t="s">
         <v>81</v>
       </c>
@@ -2908,8 +3167,11 @@
       <c r="K92" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="93" spans="3:11" x14ac:dyDescent="0.2">
+      <c r="L92" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C93" s="1" t="s">
         <v>82</v>
       </c>
@@ -2937,37 +3199,43 @@
       <c r="K93" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="94" spans="3:11" x14ac:dyDescent="0.2">
+      <c r="L93" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C94" s="1" t="s">
         <v>83</v>
       </c>
       <c r="D94" s="3">
+        <v>-4900</v>
+      </c>
+      <c r="E94" s="3">
         <v>-3900</v>
       </c>
-      <c r="E94" s="3">
+      <c r="F94" s="3">
         <v>-72500</v>
       </c>
-      <c r="F94" s="3">
+      <c r="G94" s="3">
         <v>-6900</v>
       </c>
-      <c r="G94" s="3">
+      <c r="H94" s="3">
         <v>-8500</v>
       </c>
-      <c r="H94" s="3">
+      <c r="I94" s="3">
         <v>-8000</v>
       </c>
-      <c r="I94" s="3">
+      <c r="J94" s="3">
         <v>-10700</v>
       </c>
-      <c r="J94" s="3">
+      <c r="K94" s="3">
         <v>-7300</v>
       </c>
-      <c r="K94" s="3">
+      <c r="L94" s="3">
         <v>-10200</v>
       </c>
     </row>
-    <row r="95" spans="3:11" x14ac:dyDescent="0.2">
+    <row r="95" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C95" s="1" t="s">
         <v>84</v>
       </c>
@@ -2979,8 +3247,9 @@
       <c r="I95" s="3"/>
       <c r="J95" s="3"/>
       <c r="K95" s="3"/>
-    </row>
-    <row r="96" spans="3:11" x14ac:dyDescent="0.2">
+      <c r="L95" s="3"/>
+    </row>
+    <row r="96" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C96" s="1" t="s">
         <v>85</v>
       </c>
@@ -3008,8 +3277,11 @@
       <c r="K96" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="97" spans="3:11" x14ac:dyDescent="0.2">
+      <c r="L96" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C97" s="1" t="s">
         <v>86</v>
       </c>
@@ -3037,8 +3309,11 @@
       <c r="K97" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="98" spans="3:11" x14ac:dyDescent="0.2">
+      <c r="L97" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C98" s="1" t="s">
         <v>87</v>
       </c>
@@ -3066,8 +3341,11 @@
       <c r="K98" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="99" spans="3:11" x14ac:dyDescent="0.2">
+      <c r="L98" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C99" s="1" t="s">
         <v>88</v>
       </c>
@@ -3095,37 +3373,43 @@
       <c r="K99" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="100" spans="3:11" x14ac:dyDescent="0.2">
+      <c r="L99" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C100" s="1" t="s">
         <v>89</v>
       </c>
       <c r="D100" s="3">
+        <v>2900</v>
+      </c>
+      <c r="E100" s="3">
         <v>-2400</v>
       </c>
-      <c r="E100" s="3">
+      <c r="F100" s="3">
         <v>92000</v>
       </c>
-      <c r="F100" s="3">
+      <c r="G100" s="3">
         <v>-1000</v>
       </c>
-      <c r="G100" s="3">
+      <c r="H100" s="3">
         <v>8500</v>
       </c>
-      <c r="H100" s="3">
+      <c r="I100" s="3">
         <v>8900</v>
       </c>
-      <c r="I100" s="3">
+      <c r="J100" s="3">
         <v>8200</v>
       </c>
-      <c r="J100" s="3">
+      <c r="K100" s="3">
         <v>-800</v>
       </c>
-      <c r="K100" s="3">
+      <c r="L100" s="3">
         <v>21200</v>
       </c>
     </row>
-    <row r="101" spans="3:11" x14ac:dyDescent="0.2">
+    <row r="101" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C101" s="1" t="s">
         <v>90</v>
       </c>
@@ -3153,33 +3437,39 @@
       <c r="K101" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="102" spans="3:11" x14ac:dyDescent="0.2">
+      <c r="L101" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="102" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C102" s="1" t="s">
         <v>91</v>
       </c>
       <c r="D102" s="3">
+        <v>-6100</v>
+      </c>
+      <c r="E102" s="3">
         <v>-3000</v>
       </c>
-      <c r="E102" s="3">
+      <c r="F102" s="3">
         <v>500</v>
       </c>
-      <c r="F102" s="3">
+      <c r="G102" s="3">
         <v>-2600</v>
       </c>
-      <c r="G102" s="3">
+      <c r="H102" s="3">
         <v>5600</v>
       </c>
-      <c r="H102" s="3">
+      <c r="I102" s="3">
         <v>4900</v>
       </c>
-      <c r="I102" s="3">
+      <c r="J102" s="3">
         <v>1900</v>
       </c>
-      <c r="J102" s="3">
+      <c r="K102" s="3">
         <v>-9300</v>
       </c>
-      <c r="K102" s="3">
+      <c r="L102" s="3">
         <v>6000</v>
       </c>
     </row>

</xml_diff>